<commit_message>
rest of table 1 added
</commit_message>
<xml_diff>
--- a/tutorials/oscillator/tableS1.xlsx
+++ b/tutorials/oscillator/tableS1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="49">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -130,10 +130,43 @@
     <t xml:space="preserve">produce_CApAq</t>
   </si>
   <si>
+    <t xml:space="preserve">CATCACTATCAATCCTACATCTTTTCCTAATCCCAATCAACACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTAAAGAAGAGTGGTGTGAAGATAGGAAAGGTGTTGATTGGGATTAGGAAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">....................((((((((((((((((((((((((+......................((((((((((((((((((((((+.......))))))))))))))))))))))))))))))))))))))))))))))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">....................((((((((((((((((((((((((+((((((((((((((((((((((...............+)))))))))))))))))))))).......))))))))))))))))))))))))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTCCTAATCCCAATCAACACCTTTCCTA</t>
+  </si>
+  <si>
     <t xml:space="preserve">produce_ABrBs</t>
   </si>
   <si>
+    <t xml:space="preserve">CCCATTTCTCTAACTAACCACCCTATACCCTTCTTATCCAACCG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGTGATGCGGTAATGTAAGTTTGGTATAGCGGTTGGATAAGAAGGGTATAGGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTATACCCTTCTTATCCAACCGCTATACC</t>
+  </si>
+  <si>
     <t xml:space="preserve">produce_BCjCk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCTTTACTCCTTCAACTCTCCAAACAACATCCTCACACAAACGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAATGGGCGGTGGAGGGAAGATTGTTGTTGCGTTTGTGTGAGGATGTTGTTTG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AACAACATCCTCACACAAACGCAACAACA</t>
   </si>
 </sst>
 </file>
@@ -263,15 +296,15 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="45.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="59.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="69.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="59.33"/>
@@ -645,6 +678,21 @@
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="H11" s="1" t="n">
         <v>25</v>
       </c>
@@ -665,6 +713,21 @@
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" s="1" t="n">
         <v>25</v>
       </c>
@@ -685,6 +748,21 @@
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H13" s="1" t="n">
         <v>25</v>
       </c>
@@ -700,11 +778,26 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="H14" s="1" t="n">
         <v>25</v>
       </c>
@@ -720,11 +813,26 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H15" s="1" t="n">
         <v>25</v>
       </c>
@@ -740,11 +848,26 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H16" s="1" t="n">
         <v>25</v>
       </c>
@@ -760,11 +883,26 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="H17" s="1" t="n">
         <v>25</v>
       </c>
@@ -780,11 +918,26 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H18" s="1" t="n">
         <v>25</v>
       </c>
@@ -800,10 +953,25 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>25</v>

</xml_diff>